<commit_message>
SP and process file
</commit_message>
<xml_diff>
--- a/Doc/LOAN_CL.xlsx
+++ b/Doc/LOAN_CL.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>CTG 1</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>C</t>
-  </si>
-  <si>
-    <t>195</t>
   </si>
   <si>
     <t>Jashore Branch</t>
@@ -549,7 +546,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,34 +565,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="9" t="s">
         <v>19</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -603,13 +600,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="5">
+        <v>19</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="E2" s="7">
         <v>1222</v>
@@ -624,9 +621,11 @@
         <v>2</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -635,11 +634,11 @@
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="5">
+        <v>19</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="E3" s="7">
         <v>1290</v>
@@ -654,9 +653,11 @@
         <v>3</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -665,11 +666,11 @@
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="5">
+        <v>19</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="E4" s="7">
         <v>2003</v>
@@ -684,9 +685,11 @@
         <v>4</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>